<commit_message>
Extended airport model added
</commit_message>
<xml_diff>
--- a/Airport/Flights.xlsx
+++ b/Airport/Flights.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/allen/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{363A5366-D72D-EA45-A811-9A570DC47EC6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="125" yWindow="150" windowWidth="20260" windowHeight="11057"/>
+    <workbookView xWindow="120" yWindow="460" windowWidth="23700" windowHeight="13680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -64,11 +70,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,7 +173,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Обычный_Лист1" xfId="1"/>
+    <cellStyle name="Обычный_Лист1" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -225,7 +231,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -257,9 +263,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -291,6 +315,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -466,20 +508,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScale="191" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" customWidth="1"/>
-    <col min="2" max="2" width="19.109375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="17.5" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -490,7 +532,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -498,128 +540,128 @@
         <v>42359.555555555555</v>
       </c>
       <c r="C2" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="6">
-        <v>42359.579861111109</v>
+        <v>42359.555555555555</v>
       </c>
       <c r="C3" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="6">
-        <v>42359.631944444445</v>
+        <v>42359.555555555555</v>
       </c>
       <c r="C4" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="6">
-        <v>42359.673611111109</v>
+        <v>42359.555555555555</v>
       </c>
       <c r="C5" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="6">
-        <v>42359.6875</v>
+        <v>42359.59375</v>
       </c>
       <c r="C6" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="6">
-        <v>42359.71875</v>
+        <v>42359.59375</v>
       </c>
       <c r="C7" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="6">
-        <v>42359.739583333336</v>
+        <v>42359.59375</v>
       </c>
       <c r="C8" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="6">
-        <v>42359.777777777781</v>
+        <v>42359.59375</v>
       </c>
       <c r="C9" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="6">
-        <v>42359.809027777781</v>
+        <v>42359.614583333336</v>
       </c>
       <c r="C10" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="6">
-        <v>42359.854166666664</v>
+        <v>42359.614583333336</v>
       </c>
       <c r="C11" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="6">
-        <v>42359.895833333336</v>
+        <v>42359.614583333336</v>
       </c>
       <c r="C12" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="6">
-        <v>42359.930555555555</v>
+        <v>42359.708333333336</v>
       </c>
       <c r="C13" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>